<commit_message>
Build table using list + filename to sheet name
1) Use list to build the table instead of appending
rows directly to DataFrame.
(More effective + compatible with Pandas 2.0.)

2. Sheet names contain files instead of 'okres'
</commit_message>
<xml_diff>
--- a/data/vystup.xlsx
+++ b/data/vystup.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OkresCZ0722" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OkresCZ072x" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="demo-data_okres0722" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="demo-data_okres07x" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>